<commit_message>
Ajustes gitignore y cambios menores
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library-QA\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRUEBA_AUTOMATIZACION\ORQUESTADOR\SegurosAlfa\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE21083-3D52-41D1-8225-9F8B55D7E5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D54061E-6050-409F-9B90-A9EBBA1949F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3605D7C7-CEB4-4E4A-B47F-A33611BAA749}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="788" xr2:uid="{86D55D2F-AD4D-43EC-ACA8-2638F0B3E793}"/>
   </bookViews>
   <sheets>
-    <sheet name="Inicio" sheetId="1" r:id="rId1"/>
+    <sheet name="Inicio" sheetId="10" r:id="rId1"/>
+    <sheet name="op" sheetId="4" state="hidden" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Producto">#REF!</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,39 +40,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Parametro Uno</t>
-  </si>
-  <si>
-    <t>Parametro Dos</t>
-  </si>
-  <si>
-    <t>Texto de prueba</t>
-  </si>
-  <si>
-    <t>Texto dos de prueba</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>op</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>generarEvidencia</t>
+  </si>
+  <si>
+    <t>usuario</t>
+  </si>
+  <si>
+    <t>contrasenna</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,8 +111,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -113,39 +145,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -197,7 +229,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -308,6 +340,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -316,13 +355,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -387,64 +419,80 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27691BCF-5E7F-43E9-94B5-7C23760E1AA0}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A00FF7-1EE1-471D-B4AA-405E894BC20D}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:XFD1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181DD163-2658-4783-B730-4821D74DF7F5}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>